<commit_message>
add ceckers to main
</commit_message>
<xml_diff>
--- a/Date.xlsx
+++ b/Date.xlsx
@@ -2,6 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
+  <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0"/>
   </bookViews>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="9">
   <si>
     <t>asd</t>
   </si>
@@ -26,6 +27,21 @@
   </si>
   <si>
     <t>sdasa</t>
+  </si>
+  <si>
+    <t>dfbn</t>
+  </si>
+  <si>
+    <t>sfgn</t>
+  </si>
+  <si>
+    <t>Checkers</t>
+  </si>
+  <si>
+    <t>srfgn</t>
+  </si>
+  <si>
+    <t>wrh</t>
   </si>
 </sst>
 </file>
@@ -35,7 +51,7 @@
   <numFmts count="0"/>
   <fonts count="1">
     <font>
-      <name val="Arial"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <color theme="1"/>
       <sz val="11"/>
@@ -66,7 +82,7 @@
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
 </styleSheet>
@@ -361,15 +377,15 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:F4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="14.25"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -386,7 +402,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
+    <row r="2" spans="1:6">
       <c r="A2" t="s">
         <v>3</v>
       </c>
@@ -401,6 +417,46 @@
       </c>
       <c r="E2" t="s">
         <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D3" t="n">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>8</v>
+      </c>
+      <c r="C4" t="n">
+        <v>0</v>
+      </c>
+      <c r="D4" t="n">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>2</v>
+      </c>
+      <c r="F4" t="s">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>